<commit_message>
Se arreglo un problema en la edicion de usuarios cuando el correo ya ha sido registrado. Se agrego la vista de acceso restringido. Se agrego mensajes para las operaciones de los CRUD por medio de la clase Flash de Laracast.
</commit_message>
<xml_diff>
--- a/database/mis_registros/carreras.xlsx
+++ b/database/mis_registros/carreras.xlsx
@@ -228,9 +228,6 @@
     <t>Técnico en Laboratorio Clínico</t>
   </si>
   <si>
-    <t>Ingeniería de Sistemas Informáticas</t>
-  </si>
-  <si>
     <t>Licenciatura en Ciencias del Lenguaje y la Literatura</t>
   </si>
   <si>
@@ -268,6 +265,9 @@
   </si>
   <si>
     <t>Profesorado en Matemática</t>
+  </si>
+  <si>
+    <t>Ingeniería de Sistemas Informáticos</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1076,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1100,7 +1102,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -1125,7 +1127,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
@@ -1175,7 +1177,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
@@ -1260,7 +1262,7 @@
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
@@ -1300,7 +1302,7 @@
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
@@ -1335,7 +1337,7 @@
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
@@ -1425,7 +1427,7 @@
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
@@ -1435,22 +1437,22 @@
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
@@ -1460,17 +1462,17 @@
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>